<commit_message>
Improve Word ICD extraction
</commit_message>
<xml_diff>
--- a/DECS Excel Add-Ins/test files/patient_addresses.xlsx
+++ b/DECS Excel Add-Ins/test files/patient_addresses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DECS-Office-AddIns\DECS Excel Add-Ins\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF53C5C-82DE-4437-B7F1-309957E35193}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083948AA-4D56-4C83-9B88-D1E3E46129A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28110" windowHeight="10560" xr2:uid="{190D5A45-E44A-40A2-8D24-9006DD409F38}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Address</t>
   </si>
@@ -33,30 +33,68 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Alice B. Person</t>
-  </si>
-  <si>
-    <t>Bob C. Person</t>
-  </si>
-  <si>
     <t>480 Alta Rd, San Diego CA 92179</t>
   </si>
   <si>
-    <t>Carl D. Person</t>
-  </si>
-  <si>
     <t>201 N Broadway, Escondido CA 92025</t>
   </si>
   <si>
     <t>1173 Front St, San Diego, CA 92101</t>
+  </si>
+  <si>
+    <t>400 South Melrose Drive, Suite 108 Vista, CA 92081</t>
+  </si>
+  <si>
+    <t>233 4th Ave, Chula Vista, CA 91910</t>
+  </si>
+  <si>
+    <t>3232 Main St, Lemon Grove, CA 91945</t>
+  </si>
+  <si>
+    <t>1243 National City Blvd, National City, CA 91950</t>
+  </si>
+  <si>
+    <t>220 Euclid Ave #120, San Diego, CA 92114</t>
+  </si>
+  <si>
+    <t>Barry Barber</t>
+  </si>
+  <si>
+    <t>Alice Person</t>
+  </si>
+  <si>
+    <t>Carl Person</t>
+  </si>
+  <si>
+    <t>Diego Person</t>
+  </si>
+  <si>
+    <t>Edgar Person</t>
+  </si>
+  <si>
+    <t>Frances Person</t>
+  </si>
+  <si>
+    <t>Gail Person</t>
+  </si>
+  <si>
+    <t>Harriet Person</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,8 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,51 +441,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC20AB8-B973-4742-B7D0-09E259BAE8BC}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="5" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>